<commit_message>
Formatted numbers in data summary template. Small code fix
</commit_message>
<xml_diff>
--- a/Processing/Data Summary Template.xlsx
+++ b/Processing/Data Summary Template.xlsx
@@ -610,7 +610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -722,12 +722,6 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -738,6 +732,48 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -750,22 +786,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -786,32 +807,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -822,25 +837,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1180,20 +1183,20 @@
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="79"/>
-      <c r="J1" s="60" t="s">
+      <c r="C1" s="66"/>
+      <c r="J1" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="60"/>
+      <c r="K1" s="72"/>
     </row>
     <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="63"/>
+      <c r="C2" s="73"/>
       <c r="J2" s="43" t="s">
         <v>30</v>
       </c>
@@ -1214,10 +1217,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="60"/>
+      <c r="C4" s="72"/>
     </row>
     <row r="5" spans="1:17" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
@@ -1247,54 +1250,54 @@
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="73" t="s">
+      <c r="D9" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="74"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="61"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="11"/>
-      <c r="M9" s="73" t="s">
+      <c r="M9" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="74"/>
-      <c r="O9" s="69" t="s">
+      <c r="N9" s="61"/>
+      <c r="O9" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="57" t="s">
+      <c r="P9" s="77"/>
+      <c r="Q9" s="69" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="75" t="s">
+      <c r="D10" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="81"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="75" t="s">
+      <c r="E10" s="68"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="81"/>
-      <c r="I10" s="76"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="63"/>
       <c r="J10" s="13"/>
-      <c r="K10" s="58" t="s">
+      <c r="K10" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="67" t="s">
+      <c r="L10" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="75"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="71"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="58"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="78"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="70"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
@@ -1324,13 +1327,13 @@
       <c r="J11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="59"/>
-      <c r="L11" s="68"/>
-      <c r="M11" s="77"/>
-      <c r="N11" s="78"/>
-      <c r="O11" s="72"/>
-      <c r="P11" s="68"/>
-      <c r="Q11" s="59"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="79"/>
+      <c r="P11" s="75"/>
+      <c r="Q11" s="71"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
@@ -1348,16 +1351,16 @@
       <c r="J12" s="26"/>
       <c r="K12" s="27"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="64">
+      <c r="M12" s="55">
         <f>MAX(0,3.5-0.05*MIN(D12,G12))</f>
         <v>3.5</v>
       </c>
-      <c r="N12" s="66"/>
-      <c r="O12" s="64">
+      <c r="N12" s="57"/>
+      <c r="O12" s="55">
         <f>M12</f>
         <v>3.5</v>
       </c>
-      <c r="P12" s="65"/>
+      <c r="P12" s="56"/>
       <c r="Q12" s="45" t="s">
         <v>28</v>
       </c>
@@ -1378,16 +1381,16 @@
       <c r="J13" s="26"/>
       <c r="K13" s="28"/>
       <c r="L13" s="42"/>
-      <c r="M13" s="64">
+      <c r="M13" s="55">
         <f>MAX(0,4-0.05*MIN(D13,G13))</f>
         <v>4</v>
       </c>
-      <c r="N13" s="66"/>
-      <c r="O13" s="64">
+      <c r="N13" s="57"/>
+      <c r="O13" s="55">
         <f>M13</f>
         <v>4</v>
       </c>
-      <c r="P13" s="65"/>
+      <c r="P13" s="56"/>
       <c r="Q13" s="46" t="s">
         <v>28</v>
       </c>
@@ -1408,16 +1411,16 @@
       <c r="J14" s="26"/>
       <c r="K14" s="28"/>
       <c r="L14" s="42"/>
-      <c r="M14" s="64">
+      <c r="M14" s="55">
         <f t="shared" ref="M14" si="0">MAX(0,3.5-0.05*MIN(D14,G14))</f>
         <v>3.5</v>
       </c>
-      <c r="N14" s="66"/>
-      <c r="O14" s="64">
+      <c r="N14" s="57"/>
+      <c r="O14" s="55">
         <f>M14</f>
         <v>3.5</v>
       </c>
-      <c r="P14" s="65"/>
+      <c r="P14" s="56"/>
       <c r="Q14" s="46" t="s">
         <v>28</v>
       </c>
@@ -1438,16 +1441,16 @@
       <c r="J15" s="26"/>
       <c r="K15" s="28"/>
       <c r="L15" s="42"/>
-      <c r="M15" s="64">
+      <c r="M15" s="55">
         <f>MAX(0,4-0.05*MIN(D15,G15))</f>
         <v>4</v>
       </c>
-      <c r="N15" s="66"/>
-      <c r="O15" s="64">
+      <c r="N15" s="57"/>
+      <c r="O15" s="55">
         <f>M15</f>
         <v>4</v>
       </c>
-      <c r="P15" s="65"/>
+      <c r="P15" s="56"/>
       <c r="Q15" s="46" t="s">
         <v>28</v>
       </c>
@@ -1504,16 +1507,16 @@
       <c r="J17" s="26"/>
       <c r="K17" s="28"/>
       <c r="L17" s="42"/>
-      <c r="M17" s="64">
+      <c r="M17" s="55">
         <f>MAX(9-0.15*(MIN(D17,G17)),0)</f>
         <v>9</v>
       </c>
-      <c r="N17" s="66"/>
-      <c r="O17" s="64">
+      <c r="N17" s="57"/>
+      <c r="O17" s="55">
         <f>M17-IF(MIN(D12,G12)&gt;MIN(D17,G17),(M17-MAX(0,(9-0.15*MIN(D12,G12))))/3,0)</f>
         <v>9</v>
       </c>
-      <c r="P17" s="66"/>
+      <c r="P17" s="57"/>
       <c r="Q17" s="47">
         <f>MAX(0,L17*6)</f>
         <v>0</v>
@@ -1535,16 +1538,16 @@
       <c r="J18" s="26"/>
       <c r="K18" s="28"/>
       <c r="L18" s="42"/>
-      <c r="M18" s="64">
+      <c r="M18" s="55">
         <f>MAX(10.5-0.15*(MIN(D18,G18)),0)</f>
         <v>10.5</v>
       </c>
-      <c r="N18" s="66"/>
-      <c r="O18" s="64">
+      <c r="N18" s="57"/>
+      <c r="O18" s="55">
         <f>M18-IF(MIN(D13,G13)&gt;MIN(D18,G18),(M18-MAX(0,(10.5-0.15*MIN(D13,G13))))/3,0)</f>
         <v>10.5</v>
       </c>
-      <c r="P18" s="66"/>
+      <c r="P18" s="57"/>
       <c r="Q18" s="47">
         <f>MAX(0,L18*6)</f>
         <v>0</v>
@@ -1566,16 +1569,16 @@
       <c r="J19" s="26"/>
       <c r="K19" s="28"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="64">
+      <c r="M19" s="55">
         <f>MAX(9-0.15*(MIN(D19,G19)),0)</f>
         <v>9</v>
       </c>
-      <c r="N19" s="66"/>
-      <c r="O19" s="64">
+      <c r="N19" s="57"/>
+      <c r="O19" s="55">
         <f>M19-IF(MIN(D14,G14)&gt;MIN(D19,G19),(M19-MAX(0,(9-0.15*MIN(D14,G14))))/3,0)</f>
         <v>9</v>
       </c>
-      <c r="P19" s="66"/>
+      <c r="P19" s="57"/>
       <c r="Q19" s="47">
         <f>MAX(0,L19*6)</f>
         <v>0</v>
@@ -1597,16 +1600,16 @@
       <c r="J20" s="26"/>
       <c r="K20" s="28"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="64">
+      <c r="M20" s="55">
         <f>MAX(10.5-0.15*(MIN(D20,G20)),0)</f>
         <v>10.5</v>
       </c>
-      <c r="N20" s="66"/>
-      <c r="O20" s="64">
+      <c r="N20" s="57"/>
+      <c r="O20" s="55">
         <f>M20-IF(MIN(D15,G15)&gt;MIN(D20,G20),(M20-MAX(0,(10.5-0.15*MIN(D15,G15))))/3,0)</f>
         <v>10.5</v>
       </c>
-      <c r="P20" s="66"/>
+      <c r="P20" s="57"/>
       <c r="Q20" s="47">
         <f>MAX(0,L20*6)</f>
         <v>0</v>
@@ -1661,16 +1664,16 @@
       <c r="J22" s="41"/>
       <c r="K22" s="41"/>
       <c r="L22" s="41"/>
-      <c r="M22" s="61">
+      <c r="M22" s="58">
         <f>SUM(M12:N21)</f>
         <v>141</v>
       </c>
-      <c r="N22" s="62"/>
-      <c r="O22" s="61">
+      <c r="N22" s="59"/>
+      <c r="O22" s="58">
         <f>SUM(M12:N16,O17:P21)</f>
         <v>141</v>
       </c>
-      <c r="P22" s="62"/>
+      <c r="P22" s="59"/>
       <c r="Q22" s="48">
         <f>SUM(Q17:Q21)</f>
         <v>0</v>
@@ -1679,20 +1682,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="30">
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M9:N11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:I10"/>
     <mergeCell ref="Q9:Q11"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M22:N22"/>
@@ -1709,6 +1698,20 @@
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="O9:P11"/>
+    <mergeCell ref="M9:N11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M17:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>
@@ -1722,209 +1725,206 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="51" customWidth="1"/>
-    <col min="2" max="3" width="9" style="51"/>
-    <col min="4" max="5" width="10" style="51" customWidth="1"/>
-    <col min="6" max="6" width="9" style="51" customWidth="1"/>
-    <col min="7" max="7" width="5" style="51" customWidth="1"/>
-    <col min="8" max="9" width="9" style="51"/>
-    <col min="10" max="11" width="10" style="51" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="51"/>
+    <col min="1" max="1" width="2.5" style="49" customWidth="1"/>
+    <col min="2" max="3" width="9" style="49"/>
+    <col min="4" max="4" width="12.5" style="49" customWidth="1"/>
+    <col min="5" max="5" width="10" style="49" customWidth="1"/>
+    <col min="6" max="6" width="9" style="49" customWidth="1"/>
+    <col min="7" max="7" width="5" style="49" customWidth="1"/>
+    <col min="8" max="9" width="9" style="49"/>
+    <col min="10" max="10" width="12.5" style="49" customWidth="1"/>
+    <col min="11" max="11" width="10" style="49" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="52"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="50"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="53" t="s">
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="51" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="54" t="s">
+      <c r="C4" s="85"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="52" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="54"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="85" t="s">
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="88"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="83"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="90"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="53" t="s">
+      <c r="C8" s="85"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="89" t="s">
+      <c r="H8" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="90"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="53" t="s">
+      <c r="I8" s="85"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="51" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="91"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="54" t="s">
+      <c r="C9" s="85"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="89" t="s">
+      <c r="H9" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="90"/>
-      <c r="J9" s="91"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="54" t="s">
+      <c r="I9" s="85"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="52" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="90"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="54" t="s">
+      <c r="C10" s="85"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="89" t="s">
+      <c r="H10" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="90"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="54" t="s">
+      <c r="I10" s="85"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="52" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="90"/>
-      <c r="D11" s="91"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="54" t="s">
+      <c r="C11" s="85"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="89" t="s">
+      <c r="H11" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="90"/>
-      <c r="J11" s="91"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="54" t="s">
+      <c r="I11" s="85"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="52" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="90"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="54" t="s">
+      <c r="C12" s="85"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="89" t="s">
+      <c r="H12" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="90"/>
-      <c r="J12" s="91"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="54" t="s">
+      <c r="I12" s="85"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="52" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="83"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56" t="s">
+      <c r="C13" s="88"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="92"/>
+      <c r="F13" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="82" t="s">
+      <c r="H13" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="83"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="56" t="s">
+      <c r="I13" s="88"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="54" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:F7"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="H7:L7"/>
     <mergeCell ref="B9:D9"/>
@@ -1938,6 +1938,11 @@
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed typo in summary template
</commit_message>
<xml_diff>
--- a/Processing/Data Summary Template.xlsx
+++ b/Processing/Data Summary Template.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>High beams</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>°</t>
+  </si>
+  <si>
+    <t>Right Headlamp</t>
   </si>
 </sst>
 </file>
@@ -732,47 +735,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -786,7 +756,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -807,6 +792,42 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -826,24 +847,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1170,33 +1173,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.375" customWidth="1"/>
-    <col min="2" max="2" width="28.75" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="9" width="9.625" customWidth="1"/>
-    <col min="10" max="10" width="15.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.75" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.875" style="1" customWidth="1"/>
-    <col min="13" max="16" width="9.25" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="1" customWidth="1"/>
+    <col min="13" max="16" width="9.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="J1" s="72" t="s">
+      <c r="C1" s="80"/>
+      <c r="J1" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="72"/>
+      <c r="K1" s="61"/>
     </row>
     <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="73"/>
+      <c r="C2" s="64"/>
       <c r="J2" s="43" t="s">
         <v>30</v>
       </c>
@@ -1217,10 +1220,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="72"/>
+      <c r="C4" s="61"/>
     </row>
     <row r="5" spans="1:17" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
@@ -1250,54 +1253,54 @@
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="61"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="75"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="11"/>
-      <c r="M9" s="60" t="s">
+      <c r="M9" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="61"/>
-      <c r="O9" s="76" t="s">
+      <c r="N9" s="75"/>
+      <c r="O9" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="77"/>
-      <c r="Q9" s="69" t="s">
+      <c r="P9" s="71"/>
+      <c r="Q9" s="58" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="62" t="s">
+      <c r="D10" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="68"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="62" t="s">
+      <c r="E10" s="82"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="68"/>
-      <c r="I10" s="63"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="77"/>
       <c r="J10" s="13"/>
-      <c r="K10" s="70" t="s">
+      <c r="K10" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="74" t="s">
+      <c r="L10" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="78"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="70"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="59"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
@@ -1327,13 +1330,13 @@
       <c r="J11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="71"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="64"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="79"/>
-      <c r="P11" s="75"/>
-      <c r="Q11" s="71"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="79"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="69"/>
+      <c r="Q11" s="60"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
@@ -1351,16 +1354,16 @@
       <c r="J12" s="26"/>
       <c r="K12" s="27"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="55">
+      <c r="M12" s="65">
         <f>MAX(0,3.5-0.05*MIN(D12,G12))</f>
         <v>3.5</v>
       </c>
-      <c r="N12" s="57"/>
-      <c r="O12" s="55">
+      <c r="N12" s="67"/>
+      <c r="O12" s="65">
         <f>M12</f>
         <v>3.5</v>
       </c>
-      <c r="P12" s="56"/>
+      <c r="P12" s="66"/>
       <c r="Q12" s="45" t="s">
         <v>28</v>
       </c>
@@ -1381,16 +1384,16 @@
       <c r="J13" s="26"/>
       <c r="K13" s="28"/>
       <c r="L13" s="42"/>
-      <c r="M13" s="55">
+      <c r="M13" s="65">
         <f>MAX(0,4-0.05*MIN(D13,G13))</f>
         <v>4</v>
       </c>
-      <c r="N13" s="57"/>
-      <c r="O13" s="55">
+      <c r="N13" s="67"/>
+      <c r="O13" s="65">
         <f>M13</f>
         <v>4</v>
       </c>
-      <c r="P13" s="56"/>
+      <c r="P13" s="66"/>
       <c r="Q13" s="46" t="s">
         <v>28</v>
       </c>
@@ -1411,16 +1414,16 @@
       <c r="J14" s="26"/>
       <c r="K14" s="28"/>
       <c r="L14" s="42"/>
-      <c r="M14" s="55">
+      <c r="M14" s="65">
         <f t="shared" ref="M14" si="0">MAX(0,3.5-0.05*MIN(D14,G14))</f>
         <v>3.5</v>
       </c>
-      <c r="N14" s="57"/>
-      <c r="O14" s="55">
+      <c r="N14" s="67"/>
+      <c r="O14" s="65">
         <f>M14</f>
         <v>3.5</v>
       </c>
-      <c r="P14" s="56"/>
+      <c r="P14" s="66"/>
       <c r="Q14" s="46" t="s">
         <v>28</v>
       </c>
@@ -1441,16 +1444,16 @@
       <c r="J15" s="26"/>
       <c r="K15" s="28"/>
       <c r="L15" s="42"/>
-      <c r="M15" s="55">
+      <c r="M15" s="65">
         <f>MAX(0,4-0.05*MIN(D15,G15))</f>
         <v>4</v>
       </c>
-      <c r="N15" s="57"/>
-      <c r="O15" s="55">
+      <c r="N15" s="67"/>
+      <c r="O15" s="65">
         <f>M15</f>
         <v>4</v>
       </c>
-      <c r="P15" s="56"/>
+      <c r="P15" s="66"/>
       <c r="Q15" s="46" t="s">
         <v>28</v>
       </c>
@@ -1507,16 +1510,16 @@
       <c r="J17" s="26"/>
       <c r="K17" s="28"/>
       <c r="L17" s="42"/>
-      <c r="M17" s="55">
+      <c r="M17" s="65">
         <f>MAX(9-0.15*(MIN(D17,G17)),0)</f>
         <v>9</v>
       </c>
-      <c r="N17" s="57"/>
-      <c r="O17" s="55">
+      <c r="N17" s="67"/>
+      <c r="O17" s="65">
         <f>M17-IF(MIN(D12,G12)&gt;MIN(D17,G17),(M17-MAX(0,(9-0.15*MIN(D12,G12))))/3,0)</f>
         <v>9</v>
       </c>
-      <c r="P17" s="57"/>
+      <c r="P17" s="67"/>
       <c r="Q17" s="47">
         <f>MAX(0,L17*6)</f>
         <v>0</v>
@@ -1538,16 +1541,16 @@
       <c r="J18" s="26"/>
       <c r="K18" s="28"/>
       <c r="L18" s="42"/>
-      <c r="M18" s="55">
+      <c r="M18" s="65">
         <f>MAX(10.5-0.15*(MIN(D18,G18)),0)</f>
         <v>10.5</v>
       </c>
-      <c r="N18" s="57"/>
-      <c r="O18" s="55">
+      <c r="N18" s="67"/>
+      <c r="O18" s="65">
         <f>M18-IF(MIN(D13,G13)&gt;MIN(D18,G18),(M18-MAX(0,(10.5-0.15*MIN(D13,G13))))/3,0)</f>
         <v>10.5</v>
       </c>
-      <c r="P18" s="57"/>
+      <c r="P18" s="67"/>
       <c r="Q18" s="47">
         <f>MAX(0,L18*6)</f>
         <v>0</v>
@@ -1569,16 +1572,16 @@
       <c r="J19" s="26"/>
       <c r="K19" s="28"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="55">
+      <c r="M19" s="65">
         <f>MAX(9-0.15*(MIN(D19,G19)),0)</f>
         <v>9</v>
       </c>
-      <c r="N19" s="57"/>
-      <c r="O19" s="55">
+      <c r="N19" s="67"/>
+      <c r="O19" s="65">
         <f>M19-IF(MIN(D14,G14)&gt;MIN(D19,G19),(M19-MAX(0,(9-0.15*MIN(D14,G14))))/3,0)</f>
         <v>9</v>
       </c>
-      <c r="P19" s="57"/>
+      <c r="P19" s="67"/>
       <c r="Q19" s="47">
         <f>MAX(0,L19*6)</f>
         <v>0</v>
@@ -1600,16 +1603,16 @@
       <c r="J20" s="26"/>
       <c r="K20" s="28"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="55">
+      <c r="M20" s="65">
         <f>MAX(10.5-0.15*(MIN(D20,G20)),0)</f>
         <v>10.5</v>
       </c>
-      <c r="N20" s="57"/>
-      <c r="O20" s="55">
+      <c r="N20" s="67"/>
+      <c r="O20" s="65">
         <f>M20-IF(MIN(D15,G15)&gt;MIN(D20,G20),(M20-MAX(0,(10.5-0.15*MIN(D15,G15))))/3,0)</f>
         <v>10.5</v>
       </c>
-      <c r="P20" s="57"/>
+      <c r="P20" s="67"/>
       <c r="Q20" s="47">
         <f>MAX(0,L20*6)</f>
         <v>0</v>
@@ -1664,16 +1667,16 @@
       <c r="J22" s="41"/>
       <c r="K22" s="41"/>
       <c r="L22" s="41"/>
-      <c r="M22" s="58">
+      <c r="M22" s="62">
         <f>SUM(M12:N21)</f>
         <v>141</v>
       </c>
-      <c r="N22" s="59"/>
-      <c r="O22" s="58">
+      <c r="N22" s="63"/>
+      <c r="O22" s="62">
         <f>SUM(M12:N16,O17:P21)</f>
         <v>141</v>
       </c>
-      <c r="P22" s="59"/>
+      <c r="P22" s="63"/>
       <c r="Q22" s="48">
         <f>SUM(Q17:Q21)</f>
         <v>0</v>
@@ -1682,6 +1685,20 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="30">
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M9:N11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:I10"/>
     <mergeCell ref="Q9:Q11"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M22:N22"/>
@@ -1698,20 +1715,6 @@
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="O9:P11"/>
-    <mergeCell ref="M9:N11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M17:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>
@@ -1726,205 +1729,210 @@
   <dimension ref="B1:L13"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="49" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" style="49" customWidth="1"/>
     <col min="2" max="3" width="9" style="49"/>
-    <col min="4" max="4" width="12.5" style="49" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="49" customWidth="1"/>
     <col min="5" max="5" width="10" style="49" customWidth="1"/>
     <col min="6" max="6" width="9" style="49" customWidth="1"/>
     <col min="7" max="7" width="5" style="49" customWidth="1"/>
     <col min="8" max="9" width="9" style="49"/>
-    <col min="10" max="10" width="12.5" style="49" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="49" customWidth="1"/>
     <col min="11" max="11" width="10" style="49" customWidth="1"/>
     <col min="12" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="83"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="89"/>
       <c r="G2" s="50"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="55"/>
       <c r="F3" s="51" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="85"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="52" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="89"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="85"/>
       <c r="E5" s="53"/>
       <c r="F5" s="54"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="83"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="89"/>
       <c r="G7" s="50"/>
-      <c r="H7" s="80" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="83"/>
+      <c r="H7" s="86" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="88"/>
+      <c r="L7" s="89"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="85"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="90"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="55"/>
       <c r="F8" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="84" t="s">
+      <c r="H8" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="85"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="90"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="55"/>
       <c r="L8" s="51" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="85"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="84" t="s">
+      <c r="H9" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="85"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="91"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="56"/>
       <c r="L9" s="52" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="85"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="91"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="56"/>
       <c r="F10" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="84" t="s">
+      <c r="H10" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="85"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="92"/>
+      <c r="K10" s="56"/>
       <c r="L10" s="52" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="85"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="84" t="s">
+      <c r="H11" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="85"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="56"/>
       <c r="L11" s="52" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="85"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="91"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="56"/>
       <c r="F12" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="84" t="s">
+      <c r="H12" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="85"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="91"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="56"/>
       <c r="L12" s="52" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="88"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="92"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="57"/>
       <c r="F13" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="87" t="s">
+      <c r="H13" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="88"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="92"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="54" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="H7:L7"/>
     <mergeCell ref="B9:D9"/>
@@ -1938,11 +1946,6 @@
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>